<commit_message>
Range bar chart added
</commit_message>
<xml_diff>
--- a/BiologyCoursework/Preliminary Work/PreliminaryTest4-Gamer/GamersData.xlsx
+++ b/BiologyCoursework/Preliminary Work/PreliminaryTest4-Gamer/GamersData.xlsx
@@ -888,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L24"/>
+  <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,8 +900,8 @@
     <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -925,7 +925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>1</v>
       </c>
@@ -971,8 +971,12 @@
         <f>SUM(H5,H6)/2</f>
         <v>263.20000000000005</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <f>MAX(C5:G6)</f>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16">
         <v>2</v>
       </c>
@@ -1006,8 +1010,12 @@
         <f>SUM(I5,I6)/2</f>
         <v>73.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <f>MIN(C5:G6)</f>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -1017,7 +1025,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -1027,7 +1035,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -1051,7 +1059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1071,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -1091,7 +1099,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>2</v>
       </c>
@@ -1119,7 +1127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>3</v>
       </c>
@@ -1153,8 +1161,12 @@
         <f>SUM(H11,H12,H13,H14)/4</f>
         <v>253</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <f>MAX(C11:G14)</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16">
         <v>4</v>
       </c>
@@ -1188,8 +1200,12 @@
         <f>SUM(I11,I12,I13,I14)/4</f>
         <v>46.25</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <f>MIN(C11:G14)</f>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1199,8 +1215,8 @@
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
     </row>
-    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
         <v>0</v>
@@ -1224,7 +1240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1236,7 +1252,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>1</v>
       </c>
@@ -1264,7 +1280,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
         <v>2</v>
       </c>
@@ -1292,7 +1308,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>3</v>
       </c>
@@ -1320,7 +1336,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
         <v>4</v>
       </c>
@@ -1354,8 +1370,12 @@
         <f>SUM(H19,H21,H20,H22,H23)/5</f>
         <v>266.96000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <f>MAX(C19:G23)</f>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
         <v>5</v>
       </c>
@@ -1389,8 +1409,12 @@
         <f>SUM(I19,I20,I21,I22,I23)/5</f>
         <v>62.8</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="N23">
+        <f>MIN(C19:G23)</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>